<commit_message>
update with word like sleeping, sleepy
</commit_message>
<xml_diff>
--- a/MP_4/data_and_graph.xlsx
+++ b/MP_4/data_and_graph.xlsx
@@ -8,23 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anhnguyen/Data/CSCE438/CSCE-438/MP_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDF1CEE-20BB-7A46-B700-D68D3D3F8709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D56AD3C-7325-AC4E-AE00-6DD417328D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17280" xr2:uid="{00C4CF34-EEF5-7B47-A758-2652D4B21BAA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17240" xr2:uid="{00C4CF34-EEF5-7B47-A758-2652D4B21BAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$25</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$25</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$2:$A$25</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$25</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$2:$A$25</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$2:$B$25</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$2:$A$25</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$2:$B$25</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -127,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -139,9 +129,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -925,76 +912,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1667</c:v>
+                  <c:v>5112</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1641</c:v>
+                  <c:v>4929</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1719</c:v>
+                  <c:v>5406</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2405</c:v>
+                  <c:v>7347</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2686</c:v>
+                  <c:v>7916</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2847</c:v>
+                  <c:v>8442</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2818</c:v>
+                  <c:v>8215</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2431</c:v>
+                  <c:v>7108</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2079</c:v>
+                  <c:v>5789</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1624</c:v>
+                  <c:v>4686</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1435</c:v>
+                  <c:v>3997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1440</c:v>
+                  <c:v>3987</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1594</c:v>
+                  <c:v>4322</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1488</c:v>
+                  <c:v>4294</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1658</c:v>
+                  <c:v>4643</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1541</c:v>
+                  <c:v>4356</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1350</c:v>
+                  <c:v>4023</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1430</c:v>
+                  <c:v>4171</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1138</c:v>
+                  <c:v>3624</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1005</c:v>
+                  <c:v>3367</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>952</c:v>
+                  <c:v>2918</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1108</c:v>
+                  <c:v>3569</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1013</c:v>
+                  <c:v>2981</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1070</c:v>
+                  <c:v>3234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2748,8 +2735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2769EF7C-5BED-FC43-8B89-52B8EFF4578F}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H31" sqref="H21:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2956,17 +2943,17 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>0</v>
       </c>
       <c r="B29" s="2">
-        <v>1667</v>
+        <v>5112</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2974,7 +2961,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="2">
-        <v>1641</v>
+        <v>4929</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2982,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="2">
-        <v>1719</v>
+        <v>5406</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2990,7 +2977,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="2">
-        <v>2405</v>
+        <v>7347</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2998,7 +2985,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="2">
-        <v>2686</v>
+        <v>7916</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -3006,7 +2993,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="2">
-        <v>2847</v>
+        <v>8442</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -3014,7 +3001,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="2">
-        <v>2818</v>
+        <v>8215</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -3022,7 +3009,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="2">
-        <v>2431</v>
+        <v>7108</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -3030,7 +3017,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="2">
-        <v>2079</v>
+        <v>5789</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -3038,7 +3025,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="2">
-        <v>1624</v>
+        <v>4686</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -3046,7 +3033,7 @@
         <v>10</v>
       </c>
       <c r="B39" s="2">
-        <v>1435</v>
+        <v>3997</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -3054,7 +3041,7 @@
         <v>11</v>
       </c>
       <c r="B40" s="2">
-        <v>1440</v>
+        <v>3987</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -3062,7 +3049,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="2">
-        <v>1594</v>
+        <v>4322</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -3070,7 +3057,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="2">
-        <v>1488</v>
+        <v>4294</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -3078,7 +3065,7 @@
         <v>14</v>
       </c>
       <c r="B43" s="2">
-        <v>1658</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -3086,7 +3073,7 @@
         <v>15</v>
       </c>
       <c r="B44" s="2">
-        <v>1541</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -3094,7 +3081,7 @@
         <v>16</v>
       </c>
       <c r="B45" s="2">
-        <v>1350</v>
+        <v>4023</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -3102,7 +3089,7 @@
         <v>17</v>
       </c>
       <c r="B46" s="2">
-        <v>1430</v>
+        <v>4171</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -3110,7 +3097,7 @@
         <v>18</v>
       </c>
       <c r="B47" s="2">
-        <v>1138</v>
+        <v>3624</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -3118,7 +3105,7 @@
         <v>19</v>
       </c>
       <c r="B48" s="2">
-        <v>1005</v>
+        <v>3367</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -3126,7 +3113,7 @@
         <v>20</v>
       </c>
       <c r="B49" s="2">
-        <v>952</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -3134,7 +3121,7 @@
         <v>21</v>
       </c>
       <c r="B50" s="2">
-        <v>1108</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -3142,7 +3129,7 @@
         <v>22</v>
       </c>
       <c r="B51" s="2">
-        <v>1013</v>
+        <v>2981</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -3150,13 +3137,12 @@
         <v>23</v>
       </c>
       <c r="B52" s="2">
-        <v>1070</v>
+        <v>3234</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>